<commit_message>
feat: aprimorar conversão de Excel para JSON com processamento de dados e novas entradas
</commit_message>
<xml_diff>
--- a/gerar_html/prescricoes.xlsx
+++ b/gerar_html/prescricoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1AC289667D0E8CCD/Documentos/Saúde/Prescrições/Prescrição_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1694" documentId="13_ncr:1_{243FE48A-7C6A-41E4-8FFF-32D7F4E6C3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAF53786-BDAD-400B-94FA-1D8AC13C8C64}"/>
+  <xr:revisionPtr revIDLastSave="2023" documentId="13_ncr:1_{243FE48A-7C6A-41E4-8FFF-32D7F4E6C3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC64DD7A-BEF4-48B7-BABF-A45803C220B0}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{4C639DE4-733A-4E7F-8720-AC3921A2C161}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="5" activeTab="7" xr2:uid="{4C639DE4-733A-4E7F-8720-AC3921A2C161}"/>
   </bookViews>
   <sheets>
     <sheet name="Medicamentos" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Procedimentos" sheetId="3" r:id="rId5"/>
     <sheet name="Orientacoes" sheetId="4" r:id="rId6"/>
     <sheet name="Outros" sheetId="5" r:id="rId7"/>
+    <sheet name="PortaEInternacao" sheetId="10" r:id="rId8"/>
+    <sheet name="ViasDeAdministracao" sheetId="8" r:id="rId9"/>
+    <sheet name="Aprazamentos" sheetId="9" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Renovação_receita" localSheetId="6">Outros!$D$3</definedName>
@@ -44,8 +47,147 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="3">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="3">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+    <bk>
+      <rc t="2" v="2"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
+<file path=xl/python.xml><?xml version="1.0" encoding="utf-8"?>
+<python xmlns="http://schemas.microsoft.com/office/spreadsheetml/2023/python">
+  <environmentDefinition id="{882DD1B0-6546-4DFA-8A08-902A380B44EA}">
+    <initialization>
+      <code xml:space="preserve">import numpy as np
+import pandas as pd
+import matplotlib.pyplot as plt
+import seaborn as sns
+import statsmodels as sm
+import excel
+import warnings
+warnings.simplefilter('ignore')
+excel.set_xl_scalar_conversion(excel.convert_to_scalar)
+excel.set_xl_array_conversion(excel.convert_to_dataframe)
+</code>
+    </initialization>
+  </environmentDefinition>
+  <pythonScripts>
+    <pythonScript>
+      <code>[
+  {
+    "nome": "Ceftriaxona 1g 12/12h",
+    "texto": "Ceftriaxona 1g, 1g (1 frasco), EV, 12/12h",
+    "componentes": [
+      {
+        "item": "Cloreto de sódio à 0,9%%",
+        "dose": "100",
+        "unidade": "ml"
+      }
+    ]
+  },
+  {
+    "nome": "Ceftriaxona 2g 24/24h",
+    "texto": "Ceftriaxona 1g, 2g (2 frascos), EV, 24/24h"
+  }
+]</code>
+    </pythonScript>
+    <pythonScript>
+      <code>[
+  {
+    "nome": "Fentanil 10 mcg BIC",
+    "texto": "Fentanil 50 mcg/ml, 20 ml, BIC, vazão ACM. Concentração: 10 mcg/ml",
+    "componentes":[
+      {
+        "item": "Glicose à 5%%",
+        "dose": "80",
+        "unidade": "ml"
+      }
+                  ]
+  },
+]</code>
+    </pythonScript>
+    <pythonScript>
+      <code>[
+    {
+    "nome": "Midazolam 1 mg/ml BIC (150 ml)",
+    "texto": "Midazolam 5 mg/ml, 30 ml, BIC, vazão ACM. Concentração: 1 mg/ml",
+    "componentes":[
+      {
+        "item": "SF 0,9%% ou SG 5%%",
+        "dose": "120",
+        "unidade": "ml"
+      }
+                  ]
+    },
+    {
+    "nome": "Midazolam 1 mg/ml BIC (250ml)",
+    "texto": "Midazolam 5 mg/ml, 50 ml, BIC, vazão ACM. Concentração: 1 mg/ml",
+    "componentes":[
+        {
+        "item": "SF 0,9%% ou SG 5%%",
+        "dose": "200",
+        "unidade": "ml"
+        }
+                    ]
+    },
+]</code>
+    </pythonScript>
+  </pythonScripts>
+</python>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="633">
   <si>
     <t>NomeBusca</t>
   </si>
@@ -2156,6 +2298,304 @@
   <si>
     <t>solução para nebulização</t>
   </si>
+  <si>
+    <t>1 - Loratadina 1 mg/ml ___________________ 1 frasco
+Dar ___ mls por dia</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>VO</t>
+  </si>
+  <si>
+    <t>Via oral</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>Endovenoso</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>Imtramuscular</t>
+  </si>
+  <si>
+    <t>Via inalatória</t>
+  </si>
+  <si>
+    <t>Via SNE</t>
+  </si>
+  <si>
+    <t>Via sondanasoentérica</t>
+  </si>
+  <si>
+    <t>Tópico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigla </t>
+  </si>
+  <si>
+    <t>Horário</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ItemPrincipal</t>
+  </si>
+  <si>
+    <t>TipoItem</t>
+  </si>
+  <si>
+    <t>Apresentacoes</t>
+  </si>
+  <si>
+    <t>UnidadesDose</t>
+  </si>
+  <si>
+    <t>DescricaoCompleta</t>
+  </si>
+  <si>
+    <t>PrescricoesPadronizadasJSON</t>
+  </si>
+  <si>
+    <t>ObservacaoPadrao</t>
+  </si>
+  <si>
+    <t>Medicamento</t>
+  </si>
+  <si>
+    <t>Complexo</t>
+  </si>
+  <si>
+    <t>Dieta via oral conforme prescrição nutricional</t>
+  </si>
+  <si>
+    <t>Simples</t>
+  </si>
+  <si>
+    <t>1g/frasco</t>
+  </si>
+  <si>
+    <t>g; mg</t>
+  </si>
+  <si>
+    <t>Dieta via oral</t>
+  </si>
+  <si>
+    <t>Monitorização</t>
+  </si>
+  <si>
+    <t>Cuidados da enfermagem</t>
+  </si>
+  <si>
+    <t>Sinais vitais</t>
+  </si>
+  <si>
+    <t>Sinais vitais de 2 em 2 horas</t>
+  </si>
+  <si>
+    <t>Sinais vitais de 6 em 6 horas</t>
+  </si>
+  <si>
+    <t>Via EV: Correr em 30 minutos</t>
+  </si>
+  <si>
+    <t>25 mg Comp;
+50 mg Comp</t>
+  </si>
+  <si>
+    <t>mg; Comp</t>
+  </si>
+  <si>
+    <t>Fentanil</t>
+  </si>
+  <si>
+    <t>mcg; ml</t>
+  </si>
+  <si>
+    <t>Dieta</t>
+  </si>
+  <si>
+    <t>Midazolam</t>
+  </si>
+  <si>
+    <t>5 mg/ml Amp 3 ml;
+5 mg/ml Amp 10 ml</t>
+  </si>
+  <si>
+    <t>50 mcg/ml Amp 2 ml;
+50 mcg/ml Amp 2 ml</t>
+  </si>
+  <si>
+    <t>mg; ml</t>
+  </si>
+  <si>
+    <t>Cloreto de sódio</t>
+  </si>
+  <si>
+    <t>ml; frasco</t>
+  </si>
+  <si>
+    <t>0,9% (100 ml);
+0,9% (250 ml);
+0,9% (500 ml);
+0,9% (1000 ml);</t>
+  </si>
+  <si>
+    <t>Cuidados com posicionamento</t>
+  </si>
+  <si>
+    <t>Cabeceira elevada em 30°</t>
+  </si>
+  <si>
+    <t>Prevenção de úlcera de pressão</t>
+  </si>
+  <si>
+    <t>Mudança de posição de 6 em 6 horas</t>
+  </si>
+  <si>
+    <t>Oxigenoterapia</t>
+  </si>
+  <si>
+    <t>Cateter nasal à 2 L/min, se SatO2 &lt; 94%</t>
+  </si>
+  <si>
+    <t>Hipodermóclise</t>
+  </si>
+  <si>
+    <t>Inalatório</t>
+  </si>
+  <si>
+    <t>Agora</t>
+  </si>
+  <si>
+    <t>Dose única imediata</t>
+  </si>
+  <si>
+    <t>Dose única</t>
+  </si>
+  <si>
+    <t>1/1h</t>
+  </si>
+  <si>
+    <t>2/2h</t>
+  </si>
+  <si>
+    <t>3/3h</t>
+  </si>
+  <si>
+    <t>4/4h</t>
+  </si>
+  <si>
+    <t>6/6h</t>
+  </si>
+  <si>
+    <t>8/8h</t>
+  </si>
+  <si>
+    <t>12/12h</t>
+  </si>
+  <si>
+    <t>24/24h</t>
+  </si>
+  <si>
+    <t>1x dia</t>
+  </si>
+  <si>
+    <t>1 vez ao dia</t>
+  </si>
+  <si>
+    <t>2x dia</t>
+  </si>
+  <si>
+    <t>2 vezes ao dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3x dia </t>
+  </si>
+  <si>
+    <t>3 vezes ao dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4x dia </t>
+  </si>
+  <si>
+    <t>4 vezes ao dia</t>
+  </si>
+  <si>
+    <t>1x semana</t>
+  </si>
+  <si>
+    <t>1 vez por semana</t>
+  </si>
+  <si>
+    <t>2x semana</t>
+  </si>
+  <si>
+    <t>2 vezes por semana</t>
+  </si>
+  <si>
+    <t>3x semana</t>
+  </si>
+  <si>
+    <t>3 vezes por semana</t>
+  </si>
+  <si>
+    <t>De 24 em 24 horas</t>
+  </si>
+  <si>
+    <t>De 1 em 1 hora</t>
+  </si>
+  <si>
+    <t>De 2 em 2 horas</t>
+  </si>
+  <si>
+    <t>De 8 em 8 horas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De 3 em 3 horas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">De 4 em 4 horas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">De 6 em 6 horas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">De 12 em 12 horas </t>
+  </si>
+  <si>
+    <t>48/38h</t>
+  </si>
+  <si>
+    <t>De 48 em 48 horas</t>
+  </si>
+  <si>
+    <t>72/72h</t>
+  </si>
+  <si>
+    <t>De 72 em 72 horas</t>
+  </si>
+  <si>
+    <t>Via retal</t>
+  </si>
+  <si>
+    <t>Via nasal</t>
+  </si>
+  <si>
+    <t>Via otológica</t>
+  </si>
+  <si>
+    <t>Via oftálmica</t>
+  </si>
 </sst>
 </file>
 
@@ -2200,7 +2640,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2213,8 +2653,14 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2222,11 +2668,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2277,11 +2771,91 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="47">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2589,9 +3163,172 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
+<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="2">
+  <a r="2">
+    <v t="s">&lt;dict&gt;</v>
+    <v t="s">&lt;dict&gt;</v>
+  </a>
+  <a r="1">
+    <v t="s">&lt;dict&gt;</v>
+  </a>
+</arrayData>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="7">
+  <rv s="0">
+    <v>0</v>
+  </rv>
+  <rv s="1">
+    <v>list</v>
+    <v>1</v>
+    <v>0</v>
+  </rv>
+  <rv s="2">
+    <v>&lt;class 'list'&gt;</v>
+    <v>list</v>
+    <v>[{'nome': 'Ceftriaxona 1g 12/12h', 'texto': 'Ceftriaxona 1g, 1g (1 frasco), EV, 12/12h', 'componentes': [{'item': 'Cloreto de sódio à 0,9%', 'dose': '100', 'unidade': 'ml'}]}, {'nome': 'Ceftriaxona 2g 24/24h', 'texto': 'Ceftriaxona 1g, 2g (2 frascos), ...</v>
+    <v>1</v>
+    <v>2</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+  </rv>
+  <rv s="1">
+    <v>list</v>
+    <v>4</v>
+    <v>3</v>
+  </rv>
+  <rv s="2">
+    <v>&lt;class 'list'&gt;</v>
+    <v>list</v>
+    <v>[{'nome': 'Fentanil 10 mcg BIC', 'texto': 'Fentanil 50 mcg/ml, 20 ml, BIC, vazão ACM. Concentração: 10 mcg/ml', 'componentes': [{'item': 'Glicose à 5%', 'dose': '80', 'unidade': 'ml'}]}]</v>
+    <v>4</v>
+    <v>2</v>
+  </rv>
+  <rv s="2">
+    <v>&lt;class 'list'&gt;</v>
+    <v>list</v>
+    <v>[{'nome': 'Midazolam 1 mg/ml BIC (150 ml)', 'texto': 'Midazolam 5 mg/ml, 30 ml, BIC, vazão ACM. Concentração: 1 mg/ml', 'componentes': [{'item': 'SF 0,9% ou SG 5%', 'dose': '120', 'unidade': 'ml'}]}, {'nome': 'Midazolam 1 mg/ml BIC (250ml)', 'texto': '...</v>
+    <v>1</v>
+    <v>2</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
+  <s t="_array">
+    <k n="array" t="a"/>
+  </s>
+  <s t="_entity">
+    <k n="_DisplayString" t="s"/>
+    <k n="_ViewInfo" t="spb"/>
+    <k n="arrayPreview" t="r"/>
+  </s>
+  <s t="_python">
+    <k n="Python_type" t="s"/>
+    <k n="Python_typeName" t="s"/>
+    <k n="Python_str" t="s"/>
+    <k n="preview" t="r"/>
+    <k n="_Provider" t="spb"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
+<supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <spbData count="5">
+    <spb s="0">
+      <v>2</v>
+      <v>1</v>
+      <v>list</v>
+      <v>arrayPreview</v>
+    </spb>
+    <spb s="1">
+      <v>0</v>
+    </spb>
+    <spb s="2">
+      <v>https://www.anaconda.com/excel</v>
+      <v>https://res.cdn.office.net/officepysvc/prod-preview/anacondalogo.png</v>
+      <v>Python fornecido por Anaconda</v>
+    </spb>
+    <spb s="0">
+      <v>1</v>
+      <v>1</v>
+      <v>list</v>
+      <v>arrayPreview</v>
+    </spb>
+    <spb s="1">
+      <v>3</v>
+    </spb>
+  </spbData>
+</supportingPropertyBags>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="3">
+  <s>
+    <k n="drw" t="i"/>
+    <k n="dcol" t="i"/>
+    <k n="name" t="s"/>
+    <k n="array" t="s"/>
+  </s>
+  <s>
+    <k n="ArrayCardInfo" t="spb"/>
+  </s>
+  <s>
+    <k n="link" t="s"/>
+    <k n="logo" t="s"/>
+    <k n="name" t="s"/>
+  </s>
+</spbStructures>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}" name="Tabela1" displayName="Tabela1" ref="A1:V158" totalsRowShown="0">
-  <autoFilter ref="A1:V158" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}" name="Tabela1" displayName="Tabela1" ref="A1:V159" totalsRowShown="0">
+  <autoFilter ref="A1:V159" xr:uid="{D533F96B-3659-4560-ACD7-02DCC551E6A1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V158">
     <sortCondition ref="B1:B158"/>
   </sortState>
@@ -2599,10 +3336,10 @@
     <tableColumn id="7" xr3:uid="{EEA224EE-B017-42F5-A417-487E2B86AD5D}" name="ID_Item">
       <calculatedColumnFormula>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{FF9AC4B3-0AB1-43C0-813C-9F0FBFCD27C3}" name="NomeBusca" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{A4280A1D-29DF-4DF8-BAEB-74D735392255}" name="PrescricaoCompleta" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{1C09888C-F0B3-445C-96A7-59EF6CBB8977}" name="Categoria" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{E1DAEFD1-96A5-4769-95CA-789E157CF235}" name="Doenca" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FF9AC4B3-0AB1-43C0-813C-9F0FBFCD27C3}" name="NomeBusca" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A4280A1D-29DF-4DF8-BAEB-74D735392255}" name="PrescricaoCompleta" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{1C09888C-F0B3-445C-96A7-59EF6CBB8977}" name="Categoria" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{E1DAEFD1-96A5-4769-95CA-789E157CF235}" name="Doenca" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{00D107C9-5770-4523-8A77-BC2E8CCDFA3F}" name="OrdemPrioridade"/>
     <tableColumn id="6" xr3:uid="{A2A03C33-701E-4A02-84BD-0D3C40E0270C}" name="FormaFarmaceutica"/>
     <tableColumn id="8" xr3:uid="{037F36DC-527F-4AE8-A6F4-3169AA433215}" name="isCalculable"/>
@@ -2625,103 +3362,145 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9BC025B4-0C86-43DA-9BA8-AD95BA9033CF}" name="Tabela7" displayName="Tabela7" ref="A1:B20" totalsRowShown="0">
+  <autoFilter ref="A1:B20" xr:uid="{9BC025B4-0C86-43DA-9BA8-AD95BA9033CF}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CFD77929-9554-43BE-908D-A85767D19E05}" name="Horário"/>
+    <tableColumn id="2" xr3:uid="{371D9874-4C27-4E8A-9C60-1E16D092C8FD}" name="Descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7B1BCF4E-F9B8-4BCA-9A1B-734209B09515}" name="Tabela2" displayName="Tabela2" ref="A1:E6" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7B1BCF4E-F9B8-4BCA-9A1B-734209B09515}" name="Tabela2" displayName="Tabela2" ref="A1:E6" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:E6" xr:uid="{7B1BCF4E-F9B8-4BCA-9A1B-734209B09515}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{3B85112C-C948-4532-A5A9-B2DC134B2714}" name="ID_Item" dataDxfId="41">
+    <tableColumn id="5" xr3:uid="{3B85112C-C948-4532-A5A9-B2DC134B2714}" name="ID_Item" dataDxfId="44">
       <calculatedColumnFormula>ROW() - ROW(Tabela2[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{294ACE13-D92E-4E83-AE9A-884FBB3BAD21}" name="NomeBusca" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{57C4FF43-CE4E-4A4E-A745-1D12588CAE36}" name="ConteudoTexto" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{1B0E7410-6713-475C-9274-E8D53C220050}" name="Categoria" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{E775B5FA-D905-41A5-AF49-15CA3264FA30}" name="OrdemPrioridade" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{294ACE13-D92E-4E83-AE9A-884FBB3BAD21}" name="NomeBusca" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{57C4FF43-CE4E-4A4E-A745-1D12588CAE36}" name="ConteudoTexto" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{1B0E7410-6713-475C-9274-E8D53C220050}" name="Categoria" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{E775B5FA-D905-41A5-AF49-15CA3264FA30}" name="OrdemPrioridade" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F1B6F081-4196-40D7-9E1B-E18AC00A544A}" name="Tabela57" displayName="Tabela57" ref="A1:E9" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F1B6F081-4196-40D7-9E1B-E18AC00A544A}" name="Tabela57" displayName="Tabela57" ref="A1:E9" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:E9" xr:uid="{F1B6F081-4196-40D7-9E1B-E18AC00A544A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
     <sortCondition ref="E1:E9"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{255D6023-30BF-414A-B3B5-09A8AED4AD40}" name="ID_Item" dataDxfId="34">
+    <tableColumn id="5" xr3:uid="{255D6023-30BF-414A-B3B5-09A8AED4AD40}" name="ID_Item" dataDxfId="37">
       <calculatedColumnFormula>ROW() - ROW(Tabela57[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{8C75D187-576A-41EF-9BC9-337001D161C6}" name="NomeBusca" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{7A836061-FA92-4D6E-A1CB-B0A3080FF4E2}" name="ConteudoTexto" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{9C7516CD-131C-4A90-BC19-727B1919928E}" name="Categoria" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{D9BE6F3B-192E-46DB-ADBD-41AC809A383A}" name="OrdemPrioridade" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{8C75D187-576A-41EF-9BC9-337001D161C6}" name="NomeBusca" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{7A836061-FA92-4D6E-A1CB-B0A3080FF4E2}" name="ConteudoTexto" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{9C7516CD-131C-4A90-BC19-727B1919928E}" name="Categoria" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{D9BE6F3B-192E-46DB-ADBD-41AC809A383A}" name="OrdemPrioridade" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}" name="Tabela8" displayName="Tabela8" ref="A1:E6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}" name="Tabela8" displayName="Tabela8" ref="A1:E6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:E6" xr:uid="{4EB17778-C096-4FB9-8CEA-CBC90E8CC8E2}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C07F2220-FEC5-4C0B-AB14-F80860FCB6A0}" name="ID_Item" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{C07F2220-FEC5-4C0B-AB14-F80860FCB6A0}" name="ID_Item" dataDxfId="30">
       <calculatedColumnFormula>ROW() - ROW(Tabela5[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F6AB2AED-7D50-4A14-A3D8-3D697CD7C3E6}" name="NomeBusca" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{24DCE466-5828-477A-94D8-8B94F125CA52}" name="ConteudoTexto" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{544BC52C-0699-476B-9E91-F8010861B484}" name="Categoria" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{0A44EF13-A692-417E-90F4-EEE1E0C399BB}" name="OrdemPrioridade" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{F6AB2AED-7D50-4A14-A3D8-3D697CD7C3E6}" name="NomeBusca" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{24DCE466-5828-477A-94D8-8B94F125CA52}" name="ConteudoTexto" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{544BC52C-0699-476B-9E91-F8010861B484}" name="Categoria" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{0A44EF13-A692-417E-90F4-EEE1E0C399BB}" name="OrdemPrioridade" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B195B058-C443-4C22-BFDA-1A6D6B3BD53F}" name="Tabela3" displayName="Tabela3" ref="A1:D7" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B195B058-C443-4C22-BFDA-1A6D6B3BD53F}" name="Tabela3" displayName="Tabela3" ref="A1:D7" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:D7" xr:uid="{B195B058-C443-4C22-BFDA-1A6D6B3BD53F}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{30594E46-81AD-44D9-A464-0DDB2405FA5F}" name="ID_Item" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{30594E46-81AD-44D9-A464-0DDB2405FA5F}" name="ID_Item" dataDxfId="23">
       <calculatedColumnFormula>ROW() - ROW(Tabela3[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{CC635276-E45D-489A-B013-B9CB28D05F73}" name="NomeBusca" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{C4152665-161D-4E06-A92A-C044706FA22B}" name="ConteudoTexto" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{D73DEA13-D731-4A85-9704-AF815ADF8ECA}" name="Categoria" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{CC635276-E45D-489A-B013-B9CB28D05F73}" name="NomeBusca" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{C4152665-161D-4E06-A92A-C044706FA22B}" name="ConteudoTexto" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{D73DEA13-D731-4A85-9704-AF815ADF8ECA}" name="Categoria" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BF31387E-C94D-4214-90A7-3EA03A21E459}" name="Tabela4" displayName="Tabela4" ref="A1:D8" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BF31387E-C94D-4214-90A7-3EA03A21E459}" name="Tabela4" displayName="Tabela4" ref="A1:D8" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:D8" xr:uid="{BF31387E-C94D-4214-90A7-3EA03A21E459}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{B03251EF-71D3-4778-9397-49B077E4BE95}" name="ID_Item" dataDxfId="14">
+    <tableColumn id="4" xr3:uid="{B03251EF-71D3-4778-9397-49B077E4BE95}" name="ID_Item" dataDxfId="17">
       <calculatedColumnFormula>ROW() - ROW(Tabela4[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{4E29BBAD-C1D6-4B95-B61D-6D2ACC75817D}" name="NomeBusca" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{E987E83A-5D1B-4FBA-B949-173B3B767BC5}" name="ConteudoTexto" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{5CEF5F95-0ACE-4A9D-B37D-26E33FA9BC59}" name="Categoria" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{4E29BBAD-C1D6-4B95-B61D-6D2ACC75817D}" name="NomeBusca" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E987E83A-5D1B-4FBA-B949-173B3B767BC5}" name="ConteudoTexto" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{5CEF5F95-0ACE-4A9D-B37D-26E33FA9BC59}" name="Categoria" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}" name="Tabela5" displayName="Tabela5" ref="A1:E8" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}" name="Tabela5" displayName="Tabela5" ref="A1:E8" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E8" xr:uid="{913B8A45-8E4C-40E3-89AF-FB1299E38DDE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E8">
     <sortCondition ref="E1:E8"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{FE4827F2-FADA-4522-96C6-C15115BA8429}" name="ID_Item" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{FE4827F2-FADA-4522-96C6-C15115BA8429}" name="ID_Item" dataDxfId="11">
       <calculatedColumnFormula>ROW() - ROW(Tabela5[[#Headers],[ID_Item]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{2E3E19EF-E8C4-4174-A6DD-FE62A883B65B}" name="NomeBusca" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{A403427C-6D7B-4CAC-8A29-52B0496C1B55}" name="ConteudoTexto" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{495ABE71-9083-4D12-B7AF-769A1DE8A329}" name="Categoria" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{B52F07B3-9EB3-4432-9961-0DC5F0D7CABC}" name="OrdemPrioridade" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{2E3E19EF-E8C4-4174-A6DD-FE62A883B65B}" name="NomeBusca" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{A403427C-6D7B-4CAC-8A29-52B0496C1B55}" name="ConteudoTexto" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{495ABE71-9083-4D12-B7AF-769A1DE8A329}" name="Categoria" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{B52F07B3-9EB3-4432-9961-0DC5F0D7CABC}" name="OrdemPrioridade" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{ACBDBD77-4F47-4470-9066-42382BF03E43}" name="Tabela10" displayName="Tabela10" ref="A1:I13" totalsRowShown="0">
+  <autoFilter ref="A1:I13" xr:uid="{ACBDBD77-4F47-4470-9066-42382BF03E43}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{CF3203F3-4CFD-4D66-B74A-BC12D8F80FFA}" name="ID">
+      <calculatedColumnFormula>ROW() - ROW(Tabela10[[#Headers],[ID]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{F0A4A9FD-374C-4C54-BB2A-5F28D41CC94F}" name="Categoria"/>
+    <tableColumn id="3" xr3:uid="{FFABFB1D-C8F4-405B-AEE9-D9AD9763CC53}" name="ItemPrincipal"/>
+    <tableColumn id="4" xr3:uid="{A34F1342-A7E3-4126-AD78-872FBDC5E7F9}" name="TipoItem"/>
+    <tableColumn id="5" xr3:uid="{713B817B-AFCD-41AC-9811-678098C3DAA2}" name="Apresentacoes"/>
+    <tableColumn id="6" xr3:uid="{51FD07B6-C473-44E8-86E2-4ADD006B84FE}" name="UnidadesDose"/>
+    <tableColumn id="7" xr3:uid="{27DD1729-7493-4AFC-BA0D-C3C0C3F7994C}" name="DescricaoCompleta"/>
+    <tableColumn id="8" xr3:uid="{25028A68-0087-4AD4-8FAB-FDB2744115FA}" name="PrescricoesPadronizadasJSON"/>
+    <tableColumn id="9" xr3:uid="{78D527DD-27A2-4C60-B2BB-5C8F58225E77}" name="ObservacaoPadrao"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{08C68780-8D11-4E55-B88C-5F8138D4CC5D}" name="Tabela9" displayName="Tabela9" ref="A1:B12" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="A1:B12" xr:uid="{08C68780-8D11-4E55-B88C-5F8138D4CC5D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{150208FE-C1A4-49E1-81FF-1AA10AF0B961}" name="Sigla " dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{79FC3213-8BF9-487D-8478-621C9C80380A}" name="Nome" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3043,10 +3822,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE9DEBA-C453-4102-816C-FDB2AD0D57A3}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:V158"/>
+  <dimension ref="A1:V159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F147" sqref="F147"/>
+    <sheetView topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B159" sqref="B159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7423,11 +8202,217 @@
         <v>500</v>
       </c>
     </row>
+    <row r="159" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <f>ROW() - ROW(Tabela1[[#Headers],[ID_Item]])</f>
+        <v>158</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G159" t="s">
+        <v>257</v>
+      </c>
+      <c r="H159" t="s">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960A8748-E94B-4690-B759-C2243F7BF2D9}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>595</v>
+      </c>
+      <c r="B4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>596</v>
+      </c>
+      <c r="B5" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>597</v>
+      </c>
+      <c r="B6" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>598</v>
+      </c>
+      <c r="B7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>599</v>
+      </c>
+      <c r="B8" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>600</v>
+      </c>
+      <c r="B9" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>601</v>
+      </c>
+      <c r="B10" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>602</v>
+      </c>
+      <c r="B11" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>625</v>
+      </c>
+      <c r="B12" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>627</v>
+      </c>
+      <c r="B13" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>603</v>
+      </c>
+      <c r="B14" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>605</v>
+      </c>
+      <c r="B15" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>607</v>
+      </c>
+      <c r="B16" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>609</v>
+      </c>
+      <c r="B17" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B18" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>613</v>
+      </c>
+      <c r="B19" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>615</v>
+      </c>
+      <c r="B20" t="s">
+        <v>616</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8152,7 +9137,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8303,4 +9288,417 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFFD9FF-690D-4767-9960-BAF8E0E731BC}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E1" t="s">
+        <v>554</v>
+      </c>
+      <c r="F1" t="s">
+        <v>555</v>
+      </c>
+      <c r="G1" t="s">
+        <v>556</v>
+      </c>
+      <c r="H1" t="s">
+        <v>557</v>
+      </c>
+      <c r="I1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>560</v>
+      </c>
+      <c r="E2" t="s">
+        <v>563</v>
+      </c>
+      <c r="F2" t="s">
+        <v>564</v>
+      </c>
+      <c r="H2" s="12" t="e" cm="1" vm="1">
+        <f t="array" ref="H2">_xlfn._xlws.PY(0,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>576</v>
+      </c>
+      <c r="C3" t="s">
+        <v>565</v>
+      </c>
+      <c r="D3" t="s">
+        <v>562</v>
+      </c>
+      <c r="G3" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>567</v>
+      </c>
+      <c r="C5" t="s">
+        <v>568</v>
+      </c>
+      <c r="D5" t="s">
+        <v>562</v>
+      </c>
+      <c r="G5" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>567</v>
+      </c>
+      <c r="C6" t="s">
+        <v>568</v>
+      </c>
+      <c r="D6" t="s">
+        <v>562</v>
+      </c>
+      <c r="G6" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>559</v>
+      </c>
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" t="s">
+        <v>560</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>572</v>
+      </c>
+      <c r="F7" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>559</v>
+      </c>
+      <c r="C8" t="s">
+        <v>574</v>
+      </c>
+      <c r="D8" t="s">
+        <v>560</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>579</v>
+      </c>
+      <c r="F8" t="s">
+        <v>575</v>
+      </c>
+      <c r="H8" s="12" t="e" cm="1" vm="2">
+        <f t="array" ref="H8">_xlfn._xlws.PY(1,1)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>559</v>
+      </c>
+      <c r="C9" t="s">
+        <v>577</v>
+      </c>
+      <c r="D9" t="s">
+        <v>560</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="F9" t="s">
+        <v>580</v>
+      </c>
+      <c r="H9" t="e" cm="1" vm="3">
+        <f t="array" ref="H9">_xlfn._xlws.PY(2,1)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>559</v>
+      </c>
+      <c r="C10" t="s">
+        <v>581</v>
+      </c>
+      <c r="D10" t="s">
+        <v>560</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>583</v>
+      </c>
+      <c r="F10" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>567</v>
+      </c>
+      <c r="C11" t="s">
+        <v>584</v>
+      </c>
+      <c r="D11" t="s">
+        <v>562</v>
+      </c>
+      <c r="G11" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>567</v>
+      </c>
+      <c r="C12" t="s">
+        <v>586</v>
+      </c>
+      <c r="D12" t="s">
+        <v>562</v>
+      </c>
+      <c r="G12" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>ROW() - ROW(Tabela10[[#Headers],[ID]])</f>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>588</v>
+      </c>
+      <c r="C13" t="s">
+        <v>588</v>
+      </c>
+      <c r="D13" t="s">
+        <v>562</v>
+      </c>
+      <c r="G13" t="s">
+        <v>589</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAEBC3F-9249-4D7D-8804-A8B285799DAA}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>538</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>542</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>591</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>545</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>629</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>631</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>632</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>632</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>